<commit_message>
Update of the diary
</commit_message>
<xml_diff>
--- a/GuardianEye.xlsx
+++ b/GuardianEye.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t xml:space="preserve">GuardianEye</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">0 = assente</t>
   </si>
   <si>
-    <t xml:space="preserve">Presenza membri del progetto</t>
+    <t xml:space="preserve">Presenza membri del gruppo</t>
   </si>
   <si>
     <t xml:space="preserve">Totale ore</t>
@@ -70,7 +70,10 @@
     <t xml:space="preserve">Informatica 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Sistemi e reti</t>
+    <t xml:space="preserve">Sistemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storia</t>
   </si>
 </sst>
 </file>
@@ -195,59 +198,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,10 +443,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -525,7 +528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="n">
         <v>45425</v>
       </c>
@@ -546,19 +549,19 @@
       </c>
       <c r="H5" s="14" t="n">
         <f aca="false">SUM(C5:C1000)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I5" s="13" t="n">
         <f aca="false">SUM(D5:D1000)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J5" s="13" t="n">
         <f aca="false">SUM(E5:E1000)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K5" s="13" t="n">
         <f aca="false">SUM(F5:F1000)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,6 +661,66 @@
         <v>1</v>
       </c>
       <c r="F10" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="n">
+        <v>45428</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="n">
+        <v>45429</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="n">
+        <v>45429</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ora di informatica lunedi
</commit_message>
<xml_diff>
--- a/GuardianEye.xlsx
+++ b/GuardianEye.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t xml:space="preserve">GuardianEye</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">Telecomunicazioni 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italiano 1 </t>
   </si>
 </sst>
 </file>
@@ -199,8 +202,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,328 +456,408 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.2890625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="12.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="12.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="7" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="H3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
+      <c r="A5" s="13" t="n">
         <v>45425</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="14" t="n">
+      <c r="C5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15" t="n">
         <f aca="false">SUM(C5:C1000)</f>
+        <v>15</v>
+      </c>
+      <c r="I5" s="14" t="n">
+        <f aca="false">SUM(D5:D1000)</f>
+        <v>14</v>
+      </c>
+      <c r="J5" s="14" t="n">
+        <f aca="false">SUM(E5:E1000)</f>
+        <v>14</v>
+      </c>
+      <c r="K5" s="14" t="n">
+        <f aca="false">SUM(F5:F1000)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="n">
+        <v>45426</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="n">
+        <v>45426</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="n">
+        <v>45427</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="n">
+        <v>45427</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="n">
+        <v>45427</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="n">
+        <v>45428</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="n">
+        <v>45429</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="n">
+        <v>45429</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="n">
+        <v>45429</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="n">
+        <v>45429</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="n">
+        <v>45430</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="n">
+        <v>45432</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="n">
+        <v>45432</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="n">
+        <v>45432</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="13" t="n">
-        <f aca="false">SUM(D5:D1000)</f>
-        <v>10</v>
-      </c>
-      <c r="J5" s="13" t="n">
-        <f aca="false">SUM(E5:E1000)</f>
-        <v>11</v>
-      </c>
-      <c r="K5" s="13" t="n">
-        <f aca="false">SUM(F5:F1000)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
-        <v>45426</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="n">
-        <v>45426</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="n">
-        <v>45427</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
-        <v>45427</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="n">
-        <v>45427</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="n">
-        <v>45428</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="n">
-        <v>45429</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="n">
-        <v>45429</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="n">
-        <v>45429</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="n">
-        <v>45429</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="13" t="n">
+      <c r="C19" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>